<commit_message>
Reel's Expanded Storage - 3237638097 업데이트
</commit_message>
<xml_diff>
--- a/Data/Reel's Expanded Storage - 3237638097/3237638097.xlsx
+++ b/Data/Reel's Expanded Storage - 3237638097/3237638097.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Program Files (x86)\Steam\steamapps\common\RimWorld\Mods\RMK\Pull Request Here\Reel's Expanded Storage - 3237638097\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\Reel's Expanded Storage - 3237638097\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39249A68-0CBD-45E4-9232-FDE7003DB38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3528131-0939-4FF3-94B6-D8829C7A6A34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main_240925" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="533">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -162,7 +162,7 @@
     <t>ReelStorageHayBale.label</t>
   </si>
   <si>
-    <t>large chest</t>
+    <t>hay bale</t>
   </si>
   <si>
     <t>건초 더미</t>
@@ -192,7 +192,7 @@
     <t>ReelStorageLargeWoodChest.label</t>
   </si>
   <si>
-    <t>stone pile</t>
+    <t>large chest</t>
   </si>
   <si>
     <t>대형 상자</t>
@@ -222,7 +222,7 @@
     <t>ReelStorageStonePile.label</t>
   </si>
   <si>
-    <t>tanning rack</t>
+    <t>stone pile</t>
   </si>
   <si>
     <t>돌 더미</t>
@@ -252,7 +252,7 @@
     <t>ReelStorageTanningRack.label</t>
   </si>
   <si>
-    <t>weapon rack</t>
+    <t>tanning rack</t>
   </si>
   <si>
     <t>무두질대</t>
@@ -282,7 +282,7 @@
     <t>ReelStorageWeaponRack.label</t>
   </si>
   <si>
-    <t>chest</t>
+    <t>weapon rack</t>
   </si>
   <si>
     <t>무기 거치대</t>
@@ -312,7 +312,7 @@
     <t>ReelStorageWoodChest.label</t>
   </si>
   <si>
-    <t>wood pile</t>
+    <t>chest</t>
   </si>
   <si>
     <t>상자</t>
@@ -342,7 +342,7 @@
     <t>ReelStorageWoodPile.label</t>
   </si>
   <si>
-    <t>animal feeder</t>
+    <t>barrel</t>
   </si>
   <si>
     <t>나무 더미</t>
@@ -372,7 +372,7 @@
     <t>ReelStorageAnimalFeeder.label</t>
   </si>
   <si>
-    <t>bookshelf</t>
+    <t>animal feeder</t>
   </si>
   <si>
     <t>동물 먹이통</t>
@@ -426,24 +426,24 @@
     <t>ReelStorageBookshelf.label</t>
   </si>
   <si>
+    <t>bookshelf</t>
+  </si>
+  <si>
+    <t>책장</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageBookshelf.description</t>
+  </si>
+  <si>
+    <t>ReelStorageBookshelf.description</t>
+  </si>
+  <si>
     <t>A sturdy bookshelf designed to hold books and other written materials. The bookshelf is constructed from durable wood and features multiple shelves for storing books, scrolls, and documents. It is designed to keep the written materials organized and easily accessible for reading. Can be used to increase Research speed. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
 Stack size total: 20 
 Stack per tile: 10 
 Allowed items: Books</t>
   </si>
   <si>
-    <t>책장</t>
-  </si>
-  <si>
-    <t>ThingDef+ReelStorageBookshelf.description</t>
-  </si>
-  <si>
-    <t>ReelStorageBookshelf.description</t>
-  </si>
-  <si>
-    <t>large stone pile</t>
-  </si>
-  <si>
     <t>책 및 기타 서면 자료를 보관하기 위해 설계된 튼튼한 책장입니다. 책장은 내구성 있는 목재로 제작되었으며, 책, 두루마리 및 문서를 보관할 수 있는 여러 개의 선반이 있습니다. 서면 자료를 정리하고 쉽게 접근할 수 있도록 설계되었습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
 총 스택 크기: 20
 타일당 스택: 10
@@ -456,7 +456,7 @@
     <t>ReelStorageLargeStonePile.label</t>
   </si>
   <si>
-    <t>large wood pile</t>
+    <t>large stone pile</t>
   </si>
   <si>
     <t>대형 돌 더미</t>
@@ -486,7 +486,7 @@
     <t>ReelStorageLargeWoodPile.label</t>
   </si>
   <si>
-    <t>meat hook</t>
+    <t>crate</t>
   </si>
   <si>
     <t>대형 나무 더미</t>
@@ -516,7 +516,7 @@
     <t>ReelStorageMeatHook.label</t>
   </si>
   <si>
-    <t>wine rack</t>
+    <t>meat hook</t>
   </si>
   <si>
     <t>고기 걸이</t>
@@ -546,7 +546,7 @@
     <t>ReelStorageWineRack.label</t>
   </si>
   <si>
-    <t>wood crate</t>
+    <t>wine rack</t>
   </si>
   <si>
     <t>주류 보관장</t>
@@ -576,7 +576,7 @@
     <t>ReelStorageWoodCrate.label</t>
   </si>
   <si>
-    <t>barrel pallet</t>
+    <t>apparel locker</t>
   </si>
   <si>
     <t>나무 상자</t>
@@ -606,10 +606,7 @@
     <t>ReelStorageBarrelPallet.label</t>
   </si>
   <si>
-    <t>cargo container</t>
-  </si>
-  <si>
-    <t>ThingDef+ReelStorageBarrelPallet.description</t>
+    <t>barrel pallet</t>
   </si>
   <si>
     <r>
@@ -624,6 +621,9 @@
     <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
+    <t>ThingDef+ReelStorageBarrelPallet.description</t>
+  </si>
+  <si>
     <t>ReelStorageBarrelPallet.description</t>
   </si>
   <si>
@@ -645,24 +645,24 @@
     <t>ReelStorageCargoContainer.label</t>
   </si>
   <si>
+    <t>cargo container</t>
+  </si>
+  <si>
+    <t>화물 컨테이너</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageCargoContainer.description</t>
+  </si>
+  <si>
+    <t>ReelStorageCargoContainer.description</t>
+  </si>
+  <si>
     <t>A large storage container designed to hold a variety of items for long-term storage. Items stored inside will not deteriorate over time and have no impact on the beauty of their surroundings. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
 Stack size total: 128 
 Stack per tile: 14 
 Allowed items: Everything except Foods, Corpses and Chunks</t>
   </si>
   <si>
-    <t>화물 컨테이너</t>
-  </si>
-  <si>
-    <t>ThingDef+ReelStorageCargoContainer.description</t>
-  </si>
-  <si>
-    <t>ReelStorageCargoContainer.description</t>
-  </si>
-  <si>
-    <t>food shelf</t>
-  </si>
-  <si>
     <t>장기 보관을 위해 다양한 아이템을 보관하기 위해 설계된 대형 저장 컨테이너입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
 총 스택 크기: 114
 타일당 스택: 14
@@ -675,7 +675,7 @@
     <t>ReelIndustrialShelf.label</t>
   </si>
   <si>
-    <t>industrial skip</t>
+    <t>food shelf</t>
   </si>
   <si>
     <t>식품 선반</t>
@@ -705,7 +705,7 @@
     <t>ReelStorageSkip.label</t>
   </si>
   <si>
-    <t>large locker</t>
+    <t>industrial skip</t>
   </si>
   <si>
     <t>산업 폐기물 처리함</t>
@@ -735,7 +735,10 @@
     <t>ReelStorageLargeLocker.label</t>
   </si>
   <si>
-    <t>large metal crate</t>
+    <t>A larger metal locker with a window designed to keep your apparel safe, secure, and easily accessible for outfitting your colonists. Items stored inside will not deteriorate over time and have no impact on the beauty of their surroundings. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+Stack size total: 20 
+Stack per tile: 10
+Allowed items: Apparel, Armor, Headgear</t>
   </si>
   <si>
     <t>대형 사물함</t>
@@ -765,7 +768,7 @@
     <t>ReelStorageLargeMetalCrate.label</t>
   </si>
   <si>
-    <t>large wood crate</t>
+    <t>large metal crate</t>
   </si>
   <si>
     <t>대형 금속 상자</t>
@@ -795,7 +798,10 @@
     <t>ReelStorageLargeWoodCrate.label</t>
   </si>
   <si>
-    <t>locker</t>
+    <t>A compact shelf designed to hold medicine, body parts, drugs, and plant matter. Items stored inside will not deteriorate over time and have no impact on the beauty of their surroundings, however you will still need to freeze certain items.	 	\n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+Stack size total: 18 
+Stack per tile: 9 
+Allowed items: Medicine, Plant Matter, Drugs, Neutroamine, Body parts \n\n&lt;color=#0094FF&gt;Items stored can be frozen when powered.&lt;/color&gt;</t>
   </si>
   <si>
     <t>대형 나무 상자</t>
@@ -825,7 +831,7 @@
     <t>ReelStorageLocker.label</t>
   </si>
   <si>
-    <t>medicine cabinet</t>
+    <t>locker</t>
   </si>
   <si>
     <t>사물함</t>
@@ -855,10 +861,7 @@
     <t>ReelStorageMedicineCabinet.label</t>
   </si>
   <si>
-    <t>A compact shelf designed to hold medicine, body parts, drugs, and plant matter. Items stored inside will not deteriorate over time and have no impact on the beauty of their surroundings, however you will still need to freeze certain items.	 	\n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
-Stack size total: 18 
-Stack per tile: 9 
-Allowed items: Medicine, Plant Matter, Drugs, Neutroamine, Body parts \n\n&lt;color=#0094FF&gt;Items stored can be frozen if you have Simple Utilities: Fridge installed.&lt;/color&gt;</t>
+    <t>medicine cabinet</t>
   </si>
   <si>
     <t>약품 캐비닛</t>
@@ -870,16 +873,19 @@
     <t>ReelStorageMedicineCabinet.description</t>
   </si>
   <si>
+    <t>Increases work speed when placed near a workbench. One workbench can use up to two tool cabinets. This structure can also be used to store goods and valuables. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+Stack size total: 6 
+Stack per tile: 3 
+Allowed items: Metals</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageMetalCrate.label</t>
+  </si>
+  <si>
+    <t>ReelStorageMetalCrate.label</t>
+  </si>
+  <si>
     <t>metal crate</t>
-  </si>
-  <si>
-    <t>ThingDef+ReelStorageMetalCrate.label</t>
-  </si>
-  <si>
-    <t>ReelStorageMetalCrate.label</t>
-  </si>
-  <si>
-    <t>large spacer container</t>
   </si>
   <si>
     <t>금속 상자</t>
@@ -909,7 +915,7 @@
     <t>ReelStorageLargeSpacerContainer.label</t>
   </si>
   <si>
-    <t>spacer container</t>
+    <t>large spacer container</t>
   </si>
   <si>
     <t>대형 우주 컨테이너</t>
@@ -939,7 +945,7 @@
     <t>ReelStorageSpacerContainer.label</t>
   </si>
   <si>
-    <t>spacer container stack</t>
+    <t>spacer container</t>
   </si>
   <si>
     <t>우주 컨테이너</t>
@@ -969,7 +975,7 @@
     <t>ReelStorageSpacerContainerStack.label</t>
   </si>
   <si>
-    <t>spacer locker</t>
+    <t>spacer container stack</t>
   </si>
   <si>
     <t>우주 컨테이너 더미</t>
@@ -993,7 +999,7 @@
     <t>ReelStorageSpacerLocker.label</t>
   </si>
   <si>
-    <t>ThingDef+ReelStorageFridge.label</t>
+    <t>spacer locker</t>
   </si>
   <si>
     <t>우주 사물함</t>
@@ -1023,6 +1029,18 @@
 Allowed items: Manufactured, Raw Resources</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>ToolCabinet.description</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Patches.ThingDef+Dresser.description</t>
   </si>
   <si>
@@ -1032,6 +1050,18 @@
 Allowed items: Apparel</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>Dresser.description</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Patches.ThingDef+VFE_Pottery.label</t>
   </si>
   <si>
@@ -1042,6 +1072,9 @@
   </si>
   <si>
     <t>pottery</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelNewIndustrialShelf.description</t>
   </si>
   <si>
     <t>Patches.ThingDef+VFE_Pottery.description</t>
@@ -1059,6 +1092,9 @@
     <t>Patches.ThingDef+VFE_Plinth.label</t>
   </si>
   <si>
+    <t>double shelf</t>
+  </si>
+  <si>
     <t>VFE_Plinth.label</t>
   </si>
   <si>
@@ -1069,6 +1105,9 @@
   </si>
   <si>
     <t>Patches.ThingDef+VFE_Plinth.description</t>
+  </si>
+  <si>
+    <t>ReelNewIndustrialShelf.label</t>
   </si>
   <si>
     <t>VFE_Plinth.description</t>
@@ -1083,6 +1122,9 @@
     <t>Patches.ThingDef+Misc_FileCabinet.label</t>
   </si>
   <si>
+    <t>ThingDef+ReelNewIndustrialShelf.label</t>
+  </si>
+  <si>
     <t>Misc_FileCabinet.label</t>
   </si>
   <si>
@@ -1093,6 +1135,18 @@
   </si>
   <si>
     <t>Patches.ThingDef+Misc_FileCabinet.description</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>서류 보관함</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
   </si>
   <si>
     <t>Misc_FileCabinet.description</t>
@@ -1116,6 +1170,18 @@
     <t>Patches.ThingDef+Table_Wardrobe.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>장롱</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Table_Wardrobe.description</t>
   </si>
   <si>
@@ -1137,6 +1203,18 @@
     <t>Patches.ThingDef+Table_RoyalDresser.description</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="2"/>
+      </rPr>
+      <t>귀족 옷장</t>
+    </r>
+    <phoneticPr fontId="0" type="noConversion"/>
+  </si>
+  <si>
     <t>Table_RoyalDresser.description</t>
   </si>
   <si>
@@ -1158,6 +1236,12 @@
     <t>drug cabinet</t>
   </si>
   <si>
+    <t>A sealed metal container designed to keep your perishable food safe, frozen, and easily accessible for both lunch and dinner. Items stored inside will not rot over time and have no impact on the beauty of their surroundings, as long as it's powered. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+Stack size total: 12 
+Stack per tile: 6 
+Allowed items: Foods, Plant matter, Alcohol, Beverages, Musts, Hay, Condiments \n\n&lt;color=#0094FF&gt;Items stored can be frozen when powered.&lt;/color&gt;</t>
+  </si>
+  <si>
     <t>Patches.ThingDef+VFE_DrugCabinet.description</t>
   </si>
   <si>
@@ -1173,10 +1257,16 @@
     <t>Patches.ThingDef+VFE_MachiningCabinet.label</t>
   </si>
   <si>
+    <t>ReelStorageNewFridge.description</t>
+  </si>
+  <si>
     <t>VFE_MachiningCabinet.label</t>
   </si>
   <si>
     <t>machining cabinet</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageNewFridge.description</t>
   </si>
   <si>
     <t>Patches.ThingDef+VFE_MachiningCabinet.description</t>
@@ -1191,6 +1281,9 @@
 Allowed items: Steel, Components</t>
   </si>
   <si>
+    <t>ReelStorageNewFridge.label</t>
+  </si>
+  <si>
     <t>Patches.ThingDef+VFE_SmithyCabinet.label</t>
   </si>
   <si>
@@ -1198,6 +1291,9 @@
   </si>
   <si>
     <t>smithing cabinet</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageNewFridge.label</t>
   </si>
   <si>
     <t>Patches.ThingDef+VFE_SmithyCabinet.description</t>
@@ -1215,10 +1311,19 @@
     <t>Patches.ThingDef+VFE_TailorCabinet.label</t>
   </si>
   <si>
+    <t>A compact barrel designed for storage of common goods, including raw food, plant materials, medicines, textiles, and crafted resources. Prevents deterioration, but perishable items may still need freezing. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+Stack size total: 9 
+Stack per tile: 9 
+Allowed items: Raw Plants, Herbal medicine, Animal Products, Chocolate, Plant matter, Raw fish, Wort, Hemogen, Condiments</t>
+  </si>
+  <si>
     <t>VFE_TailorCabinet.label</t>
   </si>
   <si>
     <t>tailor cabinet</t>
+  </si>
+  <si>
+    <t>ReelStorageNewBarrel.description</t>
   </si>
   <si>
     <t>Patches.ThingDef+VFE_TailorCabinet.description</t>
@@ -1236,10 +1341,16 @@
     <t>Patches.ThingDef+VFE_FabricationCabinet.label</t>
   </si>
   <si>
+    <t>ThingDef+ReelStorageNewBarrel.description</t>
+  </si>
+  <si>
     <t>VFE_FabricationCabinet.label</t>
   </si>
   <si>
     <t>fabrication cabinet</t>
+  </si>
+  <si>
+    <t>ReelStorageNewBarrel.label</t>
   </si>
   <si>
     <t>Patches.ThingDef+VFE_FabricationCabinet.description</t>
@@ -1257,6 +1368,12 @@
     <t>Patches.ThingDef+VFES_AmmoCrate.label</t>
   </si>
   <si>
+    <t>A sealed metal container designed to keep your perishable food safe, frozen, and easily accessible for both lunch and dinner. Items stored inside will not rot over time and have no impact on the beauty of their surroundings, as long as it's powered. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+Stack size total: 6 
+Stack per tile: 6 
+Allowed items: Foods, Plant matter, Alcohol, Beverages, Musts, Hay, Condiments \n\n&lt;color=#0094FF&gt;Items stored can be frozen when powered.&lt;/color&gt;</t>
+  </si>
+  <si>
     <t>VFES_AmmoCrate.label</t>
   </si>
   <si>
@@ -1267,6 +1384,12 @@
   </si>
   <si>
     <t>Patches.ThingDef+VFES_AmmoCrate.description</t>
+  </si>
+  <si>
+    <t>A piece of furniture used for organising documents and records in paper form. It will help you perform research tasks faster. This structure can also be used to store research items. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+Stack size total: 6
+Stack per tile: 6 
+Allowed items: Techprints, Tech Subpersona Core, Neurotrainers, Signal chips, Empire Intel, Research papers</t>
   </si>
   <si>
     <t>VFES_AmmoCrate.description</t>
@@ -1281,6 +1404,9 @@
     <t>Patches.ThingDef+Table_IlluminatedDresser.label</t>
   </si>
   <si>
+    <t>crate stack</t>
+  </si>
+  <si>
     <t>Table_IlluminatedDresser.label</t>
   </si>
   <si>
@@ -1288,6 +1414,9 @@
   </si>
   <si>
     <t>illuminated dresser</t>
+  </si>
+  <si>
+    <t>log pile</t>
   </si>
   <si>
     <t>Patches.ThingDef+Table_IlluminatedDresser.description</t>
@@ -1305,6 +1434,9 @@
     <t>Patches.ThingDef+VVE_GarageCabinet.label</t>
   </si>
   <si>
+    <t>logs</t>
+  </si>
+  <si>
     <t>VVE_GarageCabinet.label</t>
   </si>
   <si>
@@ -1312,6 +1444,9 @@
   </si>
   <si>
     <t>garage cabinet</t>
+  </si>
+  <si>
+    <t>차고 수납장</t>
   </si>
   <si>
     <t>Patches.ThingDef+VVE_GarageCabinet.description</t>
@@ -1326,7 +1461,7 @@
 Allowed items: Car parts</t>
   </si>
   <si>
-    <t>hay bale</t>
+    <t>ThingDef+ReelStorageFridge.label</t>
   </si>
   <si>
     <t>ReelStorageFridge.label</t>
@@ -1338,220 +1473,136 @@
     <t>fridge</t>
   </si>
   <si>
+    <t>냉장고</t>
+  </si>
+  <si>
     <t>ThingDef+ReelStorageFridge.description</t>
   </si>
   <si>
     <t>ReelStorageFridge.description</t>
   </si>
   <si>
-    <t>도자기</t>
+    <t>Hay Bale</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageNewBarrel.label</t>
+  </si>
+  <si>
+    <t>Large Chest</t>
+  </si>
+  <si>
+    <t>Stone Pile</t>
+  </si>
+  <si>
+    <t>Tanning Rack</t>
+  </si>
+  <si>
+    <t>Weapon Rack</t>
+  </si>
+  <si>
+    <t>Chest</t>
+  </si>
+  <si>
+    <t>Wood Pile</t>
+  </si>
+  <si>
+    <t>Animal Feeder</t>
+  </si>
+  <si>
+    <t>식물, 신선한 농작물, 약초, 맥아즙을 보관하기 위해 설계된 소형 용기입니다. 하지만 몇몇 물품은 여전히 냉동 보관이 필요합니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
+총 스택 크기: 8
+타일당 스택: 8
+허용된 아이템: 생식물, 약초, 동물 제품, 초콜릿, 식물 재료, 생선, 맥아즙, 혈액제, 조미료</t>
+  </si>
+  <si>
+    <t>Bookshelf</t>
+  </si>
+  <si>
+    <t>A sturdy bookshelf designed to hold books and other written materials. The bookshelf is constructed from durable wood and features multiple shelves for storing books, scrolls, and documents. It is designed to keep the written materials organized and easily accessible for reading. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+Stack size total: 20 
+Stack per tile: 10 
+Allowed items: Books</t>
+  </si>
+  <si>
+    <t>Large Stone Pile</t>
+  </si>
+  <si>
+    <t>Large Wood Pile</t>
+  </si>
+  <si>
+    <t>Meat Hook</t>
+  </si>
+  <si>
+    <t>Wine Rack</t>
+  </si>
+  <si>
+    <t>Wood Crate</t>
+  </si>
+  <si>
+    <t>Barrel Pallet</t>
+  </si>
+  <si>
+    <t>A large storage container designed to hold a variety of items for long-term storage. Items stored inside will not deteriorate over time and have no impact on the beauty of their surroundings. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+Stack size total: 114 
+Stack per tile: 14 
+Allowed items: Everything except Foods, Corpses and Chunks</t>
+  </si>
+  <si>
+    <t>Cargo Container</t>
+  </si>
+  <si>
+    <t>Food Shelf</t>
+  </si>
+  <si>
+    <t>Industrial Skip</t>
+  </si>
+  <si>
+    <t>Large Locker</t>
+  </si>
+  <si>
+    <t>Large Metal Crate</t>
+  </si>
+  <si>
+    <t>Large Wood Crate</t>
+  </si>
+  <si>
+    <t>Locker</t>
+  </si>
+  <si>
+    <t>Medicine Cabinet</t>
+  </si>
+  <si>
+    <t>A compact shelf designed to hold medicine, body parts, drugs, and plant matter. Items stored inside will not deteriorate over time and have no impact on the beauty of their surroundings, however you will still need to freeze certain items. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+Stack size total: 18 
+Stack per tile: 9 
+Allowed items: Medicine, Plant Matter, Drugs, Neutroamine, Body parts</t>
+  </si>
+  <si>
+    <t>약품, 신체 부위, 약물 및 식물 재료를 보관하기 위해 설계된 소형 선반입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다. 그러나 특정 아이템은 여전히 냉동해야 합니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
+총 스택 크기: 18
+타일당 스택: 9
+허용된 아이템: 약품, 식물 재료, 약물, 뉴트로아민, 신체 부위</t>
+  </si>
+  <si>
+    <t>Metal Crate</t>
+  </si>
+  <si>
+    <t>Large Spacer Container</t>
+  </si>
+  <si>
+    <t>Spacer Container</t>
+  </si>
+  <si>
+    <t>Spacer Container Stack</t>
   </si>
   <si>
     <t>선박 및 식민지에서 대량의 물품과 귀중품을 저장하기 위해 설계된 세 개의 고급 컨테이너 스택입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
 총 스택 크기: 80
 타일당 스택: 20
 허용된 아이템: 음식, 시체, 조각을 제외한 모든 것</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>주추</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>예술적 형상이 새겨진 작은 주추입니다. 기타 품목을 보관할 수 있습니다. 야외에서도 보관된 물건의 손상을 방지합니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 1 
-타일당 스택: 1 
-허용된 아이템: 음식, 시체, 조각을 제외한 모든 것</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>서류 보관함</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>종이 문서나 기록물을 일목요연하게 정리할 때 쓰는 작은 가구입니다. 연구 관련 품목을 보관할 수 있습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 6
-타일당 스택: 6 
-허용된 아이템: 기술청사진, 기술검증 보조자아 핵, 신경교육 혈청, 신호 칩, 제국 첩보</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>장롱</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>의류나 그 외 여러 물건을 수납하는 커다란 장롱입니다. 설치하면 주변 모든 침대가 수면 효율이 약간 상승합니다. 침대가 받는 장롱 효과는 한 개가 최대입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 6
-타일당 스택: 3 
-허용된 아이템: 의류</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>귀족 옷장</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>순금 장식과 품위 있는 외관이 돋보이는 호화로운 옷장입니다. 침대 가까이 두면 편안함이 상승합니다. 침대가 받는 옷장 효과는 한 개가 최대입니다.의류 품목을 보관할 수 있습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 6 
-타일당 스택: 3 
-허용된 아이템: 의류</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>약물 수납장</t>
-  </si>
-  <si>
-    <t>식물, 신선한 농작물, 약초, 맥아즙을 보관하기 위해 설계된 소형 용기입니다. 하지만 몇몇 물품은 여전히 냉동 보관이 필요합니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 8
-타일당 스택: 8
-허용된 아이템: 생식물, 약초, 동물 제품, 초콜릿, 식물 재료, 생선, 맥아즙, 혈액제, 조미료</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>작업 속도에 도움을 줍니다. 약물 연구대 근처에 배치되어야 합니다. 한 작업대는 수납장 최대 두 개의 영향만 받습니다. 하지만 몇몇 물품은 여전히 냉동 보관이 필요합니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 8 
-타일당 스택: 4 
-허용된 아이템: 약품, 뉴트로아민, 식물 재료</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>기계 작업 수납장</t>
-  </si>
-  <si>
-    <t>단조 작업 수납장</t>
-  </si>
-  <si>
-    <t>재봉 작업 수납장</t>
-  </si>
-  <si>
-    <t>조립 작업 수납장</t>
-  </si>
-  <si>
-    <t>작업 속도에 도움을 줍니다. 기계 작업대 근처에 배치되어야 합니다. 한 작업대는 수납장 최대 두 개의 영향만 받습니다. 물품을 보관할 수 있습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 8 
-타일당 스택: 4 
-허용된 아이템: 강철, 부품</t>
-  </si>
-  <si>
-    <t>탄약 상자</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>탄약 상자는 탄약을 저장하는 데 유용합니다. 주변 아군들의 사격 속도를 향상시킵니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 14 
-타일당 스택: 14 
-허용된 아이템: 박격포 탄약, 탄약</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>조명이 달린 옷장</t>
-  </si>
-  <si>
-    <t>밝은 조각이 조명으로 장식 된 옷장입니다. 방을 밝히는 동안 근처의 모든 침대에 작은 편의 보너스를 제공합니다. 같은 침대 근처에 둘 이상의 옷장을 배치해도 효과는 중복되지 않습니다. 물품을 보관할 수 있습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 8 
-타일당 스택: 4 
-허용된 아이템: 의류</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>차고 수납장</t>
-  </si>
-  <si>
-    <t>다양한 크기와 기능을 가진 수많은 도구가 포함되어 있는 편리한 보관함입니다. 차고 작업대 근처에 배치하면 작업 속도가 빨라집니다. 하나의 작업대는 최대 2개의 차고 수납장을 사용할 수 있습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 12 
-타일당 스택: 6 
-허용된 아이템: 차량 부품</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>냉장고</t>
-  </si>
-  <si>
-    <t>예술 작품이 새겨진 작은 크기의 도자기입니다. 간이 제작 장소에서 만들 수 있습니다. 기타 품목을 보관할 수 있습니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 3
-타일당 스택: 3 
-허용된 아이템: 음식, 생재료</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>상하기 쉬운 음식을 안전하게 냉동 보관할 수 있도록 설계된 밀폐형 금속 용기입니다. 시간에 관계없이 안전한 음식을 먹을 수 있습니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 6 
-타일당 스택: 6 
-허용된 아이템: 음식, 식물 재료, 주류, 음료, 와인, 건초, 조미료 \n\n&lt;color=#0094FF&gt;Simple Utilities: Fridge가 설치되어 있는 경우 내부 물품을 동결보관할 수 있습니다..&lt;/color&gt;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>A sealed metal container designed to keep your perishable food safe, frozen, and easily accessible for both lunch and dinner. Items stored inside will not rot over time and have no impact on the beauty of their surroundings, as long as it's powered. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
-Stack size total: 6 
-Stack per tile: 6 
-Allowed items: Foods, Plant matter, Alcohol, Beverages, Musts, Hay, Condiments \n\n&lt;color=#0094FF&gt;Items stored can be frozen if you have Simple Utilities: Fridge installed.&lt;/color&gt;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>약품, 신체 부위, 약물 및 식물 재료를 보관하기 위해 설계된 소형 선반입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다. 그러나 특정 아이템은 여전히 냉동해야 합니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 18
-타일당 스택: 9
-허용된 아이템: 약품, 식물 재료, 약물, 뉴트로아민, 신체 부위 \n\n&lt;color=#0094FF&gt;Simple Utilities: Fridge가 설치되어 있는 경우 내부 물품을 동결보관할 수 있습니다..&lt;/color&gt;</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>정착민의 장비와 옷을 안전하게 보관하고 편안하게 갈아입을 수 있도록 설계된 고급 사물함입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 60 
-타일당 스택: 20 
-허용된 아이템: 무기, 의류</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>ToolCabinet.description</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dresser.description</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>주위 모든 침대의 편안함을 개선합니다. 한 침대는 옷장 하나의 영향만 받습니다. 의류를 보관할 수 있습니다. 야외에서도 보관된 물건의 손상을 방지합니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 4 
-타일당 스택: 2 
-허용된 아이템: 의류</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>작업 속도에 도움을 줍니다. 작업대 근처에 배치되어야 합니다. 한 작업대는 수납장 최대 두 개의 영향만 받습니다. 물품을 보관할 수 있습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 6 
-타일당 스택: 3 
-허용된 아이템: 제작품, 생재료</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>작업 속도에 도움을 줍니다. 단조 작업대 근처에 배치되어야 합니다. 한 작업대는 수납장 최대 두 개의 영향만 받습니다. 물품을 보관할 수 있습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 8 
-타일당 스택: 4 
-허용된 아이템: 금속</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>작업 속도에 도움을 줍니다. 재봉 작업대 근처에 배치되어야 합니다. 한 작업대는 수납장 최대 두 개의 영향만 받습니다. 물품을 보관할 수 있습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 8 
-타일당 스택: 4 
-허용된 아이템: 섬유, 가죽</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>작업 속도에 도움을 줍니다. 조립 작업대 근처에 배치되어야 합니다. 한 작업대는 수납장 최대 두 개의 영향만 받습니다. 물품을 보관할 수 있습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 8 
-타일당 스택: 4 
-허용된 아이템: 고급 부품, 부품, 금속</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>Dresser.description</t>
-  </si>
-  <si>
-    <t>ToolCabinet.description</t>
+  </si>
+  <si>
+    <t>Spacer Locker</t>
   </si>
   <si>
     <t>선박 및 식민지에서 장비를 안전하고 쉽게 접근할 수 있도록 보관하기 위해 설계된 고급 사물함입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
@@ -1560,128 +1611,364 @@
 허용된 아이템: 무기, 의류</t>
   </si>
   <si>
-    <t>Spacer Locker</t>
-  </si>
-  <si>
-    <t>선박 및 식민지에서 대량의 물품과 귀중품을 저장하기 위해 설계된 세 개의 고급 컨테이너 스택입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 80
-타일당 스택: 20
-허용된 아이템: 음식, 시체, 조각을 제외한 모든 것</t>
-  </si>
-  <si>
-    <t>Spacer Container Stack</t>
-  </si>
-  <si>
-    <t>Spacer Container</t>
-  </si>
-  <si>
-    <t>Large Spacer Container</t>
-  </si>
-  <si>
-    <t>Metal Crate</t>
-  </si>
-  <si>
-    <t>약품, 신체 부위, 약물 및 식물 재료를 보관하기 위해 설계된 소형 선반입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다. 그러나 특정 아이템은 여전히 냉동해야 합니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 18
-타일당 스택: 9
-허용된 아이템: 약품, 식물 재료, 약물, 뉴트로아민, 신체 부위</t>
-  </si>
-  <si>
-    <t>A compact shelf designed to hold medicine, body parts, drugs, and plant matter. Items stored inside will not deteriorate over time and have no impact on the beauty of their surroundings, however you will still need to freeze certain items. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
-Stack size total: 18 
-Stack per tile: 9 
-Allowed items: Medicine, Plant Matter, Drugs, Neutroamine, Body parts</t>
-  </si>
-  <si>
-    <t>Medicine Cabinet</t>
-  </si>
-  <si>
-    <t>Locker</t>
-  </si>
-  <si>
-    <t>Large Wood Crate</t>
-  </si>
-  <si>
-    <t>Large Metal Crate</t>
-  </si>
-  <si>
-    <t>Large Locker</t>
-  </si>
-  <si>
-    <t>Industrial Skip</t>
-  </si>
-  <si>
-    <t>Food Shelf</t>
-  </si>
-  <si>
-    <t>A large storage container designed to hold a variety of items for long-term storage. Items stored inside will not deteriorate over time and have no impact on the beauty of their surroundings. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
-Stack size total: 114 
-Stack per tile: 14 
-Allowed items: Everything except Foods, Corpses and Chunks</t>
-  </si>
-  <si>
-    <t>Cargo Container</t>
-  </si>
-  <si>
-    <t>드럼통 팔레트</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Barrel Pallet</t>
-  </si>
-  <si>
-    <t>Wood Crate</t>
-  </si>
-  <si>
-    <t>Wine Rack</t>
-  </si>
-  <si>
-    <t>Meat Hook</t>
-  </si>
-  <si>
-    <t>Large Wood Pile</t>
-  </si>
-  <si>
-    <t>Large Stone Pile</t>
-  </si>
-  <si>
-    <t>A sturdy bookshelf designed to hold books and other written materials. The bookshelf is constructed from durable wood and features multiple shelves for storing books, scrolls, and documents. It is designed to keep the written materials organized and easily accessible for reading. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+    <t>ToolCabinet.description</t>
+  </si>
+  <si>
+    <t>Dresser.description</t>
+  </si>
+  <si>
+    <t>ReelNewIndustrialShelf.description</t>
+  </si>
+  <si>
+    <t>A shelf designed to hold a wide variety of items, including meals and raw food. Items stored inside will not deteriorate over time, however you will still need to freeze certain items to prevent spoilage. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
 Stack size total: 20 
 Stack per tile: 10 
-Allowed items: Books</t>
-  </si>
-  <si>
-    <t>Bookshelf</t>
-  </si>
-  <si>
-    <t>식물, 신선한 농작물, 약초, 맥아즙을 보관하기 위해 설계된 소형 용기입니다. 하지만 몇몇 물품은 여전히 냉동 보관이 필요합니다. \n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; 
-총 스택 크기: 8
-타일당 스택: 8
-허용된 아이템: 생식물, 약초, 동물 제품, 초콜릿, 식물 재료, 생선, 맥아즙, 혈액제, 조미료</t>
-  </si>
-  <si>
-    <t>Animal Feeder</t>
-  </si>
-  <si>
-    <t>Wood Pile</t>
-  </si>
-  <si>
-    <t>Chest</t>
-  </si>
-  <si>
-    <t>Weapon Rack</t>
-  </si>
-  <si>
-    <t>Tanning Rack</t>
-  </si>
-  <si>
-    <t>Stone Pile</t>
-  </si>
-  <si>
-    <t>Large Chest</t>
-  </si>
-  <si>
-    <t>Hay Bale</t>
+Allowed items: Meals, Raw Food, Everything except Corpses and Chunks</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageNewLargeLocker.label</t>
+  </si>
+  <si>
+    <t>ReelStorageNewLargeLocker.label</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageNewLargeLocker.description</t>
+  </si>
+  <si>
+    <t>ReelStorageNewLargeLocker.description</t>
+  </si>
+  <si>
+    <t>A large metal locker with a window designed to keep your apparel safe, secure, and easily accessible for outfitting your colonists. Items stored inside will not deteriorate over time and have no impact on the beauty of their surroundings. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+Stack size total: 20 
+Stack per tile: 10
+Allowed items: Apparel, Armor, Headgear</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageNewLargeWoodCrate.label</t>
+  </si>
+  <si>
+    <t>ReelStorageNewLargeWoodCrate.label</t>
+  </si>
+  <si>
+    <t>large crate</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageNewLargeWoodCrate.description</t>
+  </si>
+  <si>
+    <t>ReelStorageNewLargeWoodCrate.description</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageNewMedicineCabinet.label</t>
+  </si>
+  <si>
+    <t>ReelStorageNewMedicineCabinet.label</t>
+  </si>
+  <si>
+    <t>medical cabinet</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageNewMedicineCabinet.description</t>
+  </si>
+  <si>
+    <t>ReelStorageNewMedicineCabinet.description</t>
+  </si>
+  <si>
+    <t>A compact shelf designed to hold medicine, body parts, drugs, and plant matter. Items stored inside will not rot over time and have no impact on the beauty of their surroundings, as long as it's powered.	 	\n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+Stack size total: 36 
+Stack per tile: 18 
+Allowed items: Medicine, Plant Matter, Drugs, Neutroamine, Body parts, Medical equipment \n\n&lt;color=#0094FF&gt;Items stored can be frozen when powered.&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageVerticalWeaponRack.label</t>
+  </si>
+  <si>
+    <t>ReelStorageVerticalWeaponRack.label</t>
+  </si>
+  <si>
+    <t>vertical weapon rack</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageVerticalWeaponRack.description</t>
+  </si>
+  <si>
+    <t>ReelStorageVerticalWeaponRack.description</t>
+  </si>
+  <si>
+    <t>A specialized rack designed to display numerous melee and ranged weapons for armories and outposts. Items stored inside will not deteriorate over time. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+Stack size total: 16 
+Stack per tile: 8 
+Allowed items: Ranged weapons, Melee weapons, Explosives</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageHorizontalWeaponRack.label</t>
+  </si>
+  <si>
+    <t>ReelStorageHorizontalWeaponRack.label</t>
+  </si>
+  <si>
+    <t>horizontal weapon rack</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageHorizontalWeaponRack.description</t>
+  </si>
+  <si>
+    <t>ReelStorageHorizontalWeaponRack.description</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageNewWoodCrate.label</t>
+  </si>
+  <si>
+    <t>ReelStorageNewWoodCrate.label</t>
+  </si>
+  <si>
+    <t>ThingDef+ReelStorageNewWoodCrate.description</t>
+  </si>
+  <si>
+    <t>ReelStorageNewWoodCrate.description</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+Shelf.description</t>
+  </si>
+  <si>
+    <t>Shelf.description</t>
+  </si>
+  <si>
+    <t>Adaptive Storage Framework &amp;&amp; Adaptive Storage Framework</t>
+  </si>
+  <si>
+    <t>A triple-stack shelf that holds three times as much as empty ground. Items stored inside will never deteriorate and don't affect the beauty of their surroundings.\n\nSince shelf space is limited, shelves cannot hold chunks, buildings, plants and large corpses. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+Stack size total: 6 
+Stack per tile: 3 
+Allowed items: Foods, Manufactured, Raw Resources, Items, Weapons, Apparel, Corpses</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+ShelfSmall.description</t>
+  </si>
+  <si>
+    <t>ShelfSmall.description</t>
+  </si>
+  <si>
+    <t>A small triple-stack shelf that holds three times as much as empty ground. Items stored inside will never deteriorate and don't affect the beauty of their surroundings.\n\nSince shelf space is limited, shelves cannot hold chunks, buildings, plants and large corpses. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+Stack size total: 3 
+Stack per tile: 3 
+Allowed items: Foods, Manufactured, Raw Resources, Items, Weapons, Apparel, Corpses</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+VFE_RoyalWardrobe.label</t>
+  </si>
+  <si>
+    <t>VFE_RoyalWardrobe.label</t>
+  </si>
+  <si>
+    <t>royal wardrobe</t>
+  </si>
+  <si>
+    <t>Patches.ThingDef+VFE_RoyalWardrobe.description</t>
+  </si>
+  <si>
+    <t>VFE_RoyalWardrobe.description</t>
+  </si>
+  <si>
+    <t>A grand, gold-trimmed wardrobe designed for nobility. Gives a small comfort bonus to all nearby beds. Placing more than one royal wardrobe near the same bed has no effect. Can be used to store Apparel. \n\n&lt;color=#E5E54C&gt;Storage stats:&lt;/color&gt; 
+Stack size total: 8 
+Stack per tile: 4 
+Allowed items: Apparel</t>
+  </si>
+  <si>
+    <t>통나무 더미</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대형 통나무 더미</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>의류함</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>나무 상자 더미</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>나무통</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>원시 시대 식민지에 적합한 저장 용기를 제작하여 물품을 보호하고, 자원을 정리하며, 무기를 전시할 수 있는 방법을 제공합니다.</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>이중 선반</t>
+  </si>
+  <si>
+    <t>의류 보관함</t>
+  </si>
+  <si>
+    <t>수직 무기 거치대</t>
+  </si>
+  <si>
+    <t>수평 무기 거치대</t>
+  </si>
+  <si>
+    <t>왕실 옷장</t>
+  </si>
+  <si>
+    <t>작은 상자에 비해 저장 용량이 늘어난 두 타일을 차지하는 대형 나무 상자입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 8\n타일당 스택: 4\n\n허용된 아이템: 음식, 시체, 조각을 제외한 모든 것</t>
+  </si>
+  <si>
+    <t>다양한 종류의 가죽과 가죽을 보관하기 위해 설계된 전문 구조물입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 12\n타일당 스택: 6\n\n허용된 아이템: 가죽</t>
+  </si>
+  <si>
+    <t>무기고 및 전초 기지에 여러 근접 및 원거리 무기를 전시하기 위해 설계된 전문 랙입니다. 내부에 저장된 아이템은 시간이 지나도 악화되지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 8\n타일당 스택: 4\n\n허용된 아이템: 근접 무기, 원거리 무기</t>
+  </si>
+  <si>
+    <t>제한된 양의 아이템을 저장하기 위해 설계된 단일 타일 나무 상자입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 4\n타일당 스택: 4\n\n허용된 아이템: 음식, 시체, 조각을 제외한 모든 것</t>
+  </si>
+  <si>
+    <t>동물들에게 먹이를 제공하기 위해 설계된 전문 저장 용기입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 18\n타일당 스택: 9\n\n허용된 아이템: 건초, 사료</t>
+  </si>
+  <si>
+    <t>책 및 기타 서면 자료를 보관하기 위해 설계된 튼튼한 책장입니다. 책장은 내구성 있는 목재로 제작되었으며, 책, 두루마리 및 문서를 보관할 수 있는 여러 개의 선반이 있습니다. 서면 자료를 정리하고 쉽게 접근할 수 있도록 설계되었습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 20\n타일당 스택: 10\n\n허용된 아이템: 책</t>
+  </si>
+  <si>
+    <t>도축 또는 처리할 생고기와 시체를 보관하기 위해 설계된 전문 랙입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다. 하지만 몇몇 물품은 여전히 냉동 보관이 필요합니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 16\n타일당 스택: 8\n\n허용된 아이템: 생고기, 생선, 시체</t>
+  </si>
+  <si>
+    <t>와인 및 기타 알코올 음료를 즐기거나 거래하기 위해 설계된 세련된 보관장입니다. 내부에 저장된 아이템은 시간이 지나도 악화되지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 10\n타일당 스택: 10\n\n허용된 아이템: 맥주, 와인, 단순 주류, 고급 주류</t>
+  </si>
+  <si>
+    <t>대량의 물품과 귀중품을 저장하기 위해 설계된 튼튼한 나무 상자입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 8\n타일당 스택: 8\n\n허용된 아이템: 음식, 시체, 조각을 제외한 모든 것</t>
+  </si>
+  <si>
+    <t>발전기, 차량 및 기타 기계에 사용되는 화학연료를 보관하기 위해 설계된 대형 저장 구조물입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 60\n타일당 스택: 15\n\n허용된 아이템: 화학연료</t>
+  </si>
+  <si>
+    <t>장기 보관을 위해 다양한 아이템을 보관하기 위해 설계된 대형 저장 컨테이너입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 114\n타일당 스택: 14\n\n허용된 아이템: 음식, 시체, 조각을 제외한 모든 것</t>
+  </si>
+  <si>
+    <t>식사, 생식품, 식물 재료, 워트를 보관하기 위해 설계된 산업용 선반입니다. 내부에 저장된 아이템은 시간이 지나도 악화되지 않지만 특정 아이템은 여전히 냉동해야 합니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 20\n타일당 스택: 10\n\n허용된 아이템: 음식, 식물 재료, 맥아즙, 약초</t>
+  </si>
+  <si>
+    <t>시체, 조각, 슬래그 및 폐기물팩을 보관하기 위해 설계된 산업용 스킵입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다. 하지만 몇몇 물품은 여전히 냉동 보관이 필요합니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 18\n타일당 스택: 9\n\n허용된 아이템: 조각, 시체, 폐기물, 재활용팩, 대변 슬러지</t>
+  </si>
+  <si>
+    <t>장비를 안전하고 쉽게 접근할 수 있도록 보관하기 위해 설계된 대형 금속 사물함입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 20\n타일당 스택: 10\n\n허용된 아이템: 의류, 갑옷, 모자</t>
+  </si>
+  <si>
+    <t>대량의 물품과 귀중품을 저장하기 위해 설계된 다섯 개의 튼튼한 금속 상자입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 52\n타일당 스택: 13\n\n허용된 아이템: 음식, 시체, 조각을 제외한 모든 것</t>
+  </si>
+  <si>
+    <t>대량의 물품과 귀중품을 저장하기 위해 설계된 여러 개의 나무 상자입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 40\n타일당 스택: 10\n\n허용된 아이템: 음식, 시체, 조각을 제외한 모든 것</t>
+  </si>
+  <si>
+    <t>장비를 안전하고 쉽게 접근할 수 있도록 보관하기 위해 설계된 금속 사물함입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 12\n타일당 스택: 12\n\n허용된 아이템: 의류, 무기</t>
+  </si>
+  <si>
+    <t>약품, 신체 부위, 약물 및 식물 재료를 보관하기 위해 설계된 소형 선반입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다. 그러나 특정 아이템은 여전히 냉동해야 합니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 18\n타일당 스택: 9\n\n허용된 아이템: 약품, 식물 재료, 약물, 뉴트로아민, 신체 부위\n\n&lt;color=#0094FF&gt;전원을 공급하면 내부 물품을 동결보관할 수 있습니다..&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>대량의 물품과 귀중품을 저장하기 위해 설계된 튼튼한 금속 상자입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 10\n타일당 스택: 10\n\n허용된 아이템: 음식, 시체, 조각을 제외한 모든 것</t>
+  </si>
+  <si>
+    <t>선박 및 식민지에서 대량의 물품과 귀중품을 저장하기 위해 설계된 고급 컨테이너입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 15\n타일당 스택: 15\n\n허용된 아이템: 음식, 시체, 조각을 제외한 모든 것</t>
+  </si>
+  <si>
+    <t>선박 및 식민지에서 대량의 물품과 귀중품을 저장하기 위해 설계된 세 개의 고급 컨테이너 스택입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 80\n타일당 스택: 20\n\n허용된 아이템: 음식, 시체, 조각을 제외한 모든 것</t>
+  </si>
+  <si>
+    <t>정착민의 장비와 옷을 안전하게 보관하고 편안하게 갈아입을 수 있도록 설계된 고급 사물함입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 60\n타일당 스택: 20\n\n허용된 아이템: 무기, 의류</t>
+  </si>
+  <si>
+    <t>작업 속도에 도움을 줍니다. 작업대 근처에 배치되어야 합니다. 한 작업대는 수납장 최대 두 개의 영향만 받습니다. 상품과 귀중품을 보관할 수 있습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 6\n타일당 스택: 3\n\n허용된 아이템: 금속</t>
+  </si>
+  <si>
+    <t>주위 모든 침대의 편안함을 개선합니다. 한 침대는 옷장 하나의 영향만 받습니다. 의류를 보관할 수 있습니다. 야외에서도 보관된 물건의 손상을 방지합니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 4\n타일당 스택: 2\n\n허용된 아이템: 의류</t>
+  </si>
+  <si>
+    <t>종이 문서나 기록물을 일목요연하게 정리할 때 쓰는 작은 가구입니다. 연구 관련 품목을 보관할 수 있습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 6\n타일당 스택: 6\n\n허용된 아이템: 기술청사진, 기술검증 보조자아 핵, 신경교육 혈청, 신호 칩, 제국 첩보</t>
+  </si>
+  <si>
+    <t>의류나 그 외 여러 물건을 수납하는 커다란 장롱입니다. 설치하면 주변 모든 침대가 수면 효율이 약간 상승합니다. 침대가 받는 장롱 효과는 한 개가 최대입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 6\n타일당 스택: 3\n\n허용된 아이템: 의류</t>
+  </si>
+  <si>
+    <t>순금 장식과 품위 있는 외관이 돋보이는 호화로운 옷장입니다. 침대 가까이 두면 편안함이 상승합니다. 침대가 받는 옷장 효과는 한 개가 최대입니다.의류 품목을 보관할 수 있습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 6\n타일당 스택: 3\n\n허용된 아이템: 의류</t>
+  </si>
+  <si>
+    <t>다양한 크기와 기능을 가진 수많은 도구가 포함되어 있는 편리한 보관함입니다. 차고 작업대 근처에 배치하면 작업 속도가 빨라집니다. 하나의 작업대는 최대 2개의 차고 수납장을 사용할 수 있습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 12\n타일당 스택: 6\n\n허용된 아이템: 차량 부품</t>
+  </si>
+  <si>
+    <t>상하기 쉬운 음식을 안전하게 냉동 보관할 수 있도록 설계된 밀폐형 금속 용기입니다. 시간에 관계없이 안전한 음식을 먹을 수 있습니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 6\n타일당 스택: 6\n\n허용된 아이템: 음식, 식물 재료, 주류, 음료, 와인, 건초, 조미료\n\n&lt;color=#0094FF&gt;전원을 공급하면 내부 물품을 동결보관할 수 있습니다..&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>귀족을 위해 설계된 웅장한 금색 장식의 옷장입니다. 근처의 모든 침대에 약간의 편안함 보너스를 제공합니다. 같은 침대 근처에 여러 개의 왕실 옷장을 배치해도 효과는 없습니다. 의류 보관에 사용할 수 있습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; \n총 스택 크기: 8\n타일당 스택: 4\n\n허용된 아이템: 의류</t>
+  </si>
+  <si>
+    <t>건초를 꼰 끈이나 밧줄로 묶어둔 압축된 더미입니다. 건초를 건조하게 유지하고 가축 및 다른 동물에게 쉽게 먹일 수 있도록 설계되었습니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 8\n타일당 스택: 8\n\n허용된 아이템: 건초</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>선박 및 식민지에서 대량의 물품과 귀중품을 저장하기 위해 설계된 더 큰 고급 컨테이너입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 30\n타일당 스택: 15\n\n허용된 아이템: 음식, 시체, 조각을 제외한 모든 것</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>빈 땅보다 세 배 많은 양을 보관할 수 있는 삼중 선반입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n선반 공간은 제한되어 있으므로 덩어리, 건물, 식물 및 대형 시체는 보관할 수 없습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; \n총 스택 크기: 6\n타일당 스택: 3\n\n허용된 아이템: 음식, 가공품, 자원, 아이템, 무기, 의류, 시체</t>
+  </si>
+  <si>
+    <t>빈 땅보다 세 배 많은 양을 보관할 수 있는 소형 삼중 선반입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n선반 공간은 제한되어 있으므로 덩어리, 건물, 식물 및 대형 시체는 보관할 수 없습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; \n총 스택 크기: 3\n타일당 스택: 3\n\n허용된 아이템: 음식, 가공품, 자원, 아이템, 무기, 의류, 시체</t>
+  </si>
+  <si>
+    <t>의류를 안전하고 확실하게 보관하며 정착민들에게 쉽게 입힐 수 있도록 설계된 창문이 있는 대형 금속 보관함입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; \n총 스택 크기: 20\n타일당 스택: 10\n\n허용된 아이템: 의류, 방어구, 머리보호대</t>
+  </si>
+  <si>
+    <t>무기고 및 전초 기지에서 다양한 근접 및 원거리 무기를 전시하도록 설계된 특수 거치대입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; \n총 스택 크기: 16\n타일당 스택: 8\n\n허용된 아이템: 원거리 무기, 근접 무기, 폭발물</t>
+  </si>
+  <si>
+    <t>상하기 쉬운 음식을 안전하고 얼린 상태로 유지하며 점심과 저녁 식사 모두에 쉽게 접근할 수 있도록 설계된 밀폐된 금속 용기입니다. 전원이 공급되는 한, 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; \n총 스택 크기: 12\n타일당 스택: 6\n\n허용된 아이템: 음식, 식물성 물질, 술, 음료, 과즙, 건초, 조미료\n\n&lt;color=#0094FF&gt;전원이 공급되면 보관된 품목을 냉동할 수 있습니다.&lt;/color&gt;</t>
+  </si>
+  <si>
+    <t>식물, 신선한 농작물, 약초, 맥아즙을 보관하기 위해 설계된 소형 용기입니다. 하지만 몇몇 물품은 여전히 냉동 보관이 필요합니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 8\n타일당 스택: 8\n\n허용된 아이템: 생식물, 약초, 동물 제품, 초콜릿, 식물 재료, 생선, 맥아즙, 혈액, 조미료</t>
+  </si>
+  <si>
+    <t>식사와 생식품을 포함한 다양한 품목을 보관하도록 설계된 선반입니다. 내부에 보관된 품목은 시간이 지나도 부패하지 않지만, 부패를 방지하려면 특정 품목은 여전히 냉동해야 합니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; \n총 스택 크기: 20\n타일당 스택: 10\n\n허용된 아이템: 식사, 생식, 시체와 덩어리를 제외한 모든 것</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>일반적인 식량, 식물성 재료, 약품, 직물, 제작된 자원 등을 보관하도록 설계된 소형 통입니다. 부패를 방지하지만, 상하기 쉬운 품목은 여전히 냉동이 필요할 수 있습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; \n총 스택 크기: 9\n타일당 스택: 9\n\n허용된 아이템: 식물, 약초, 동물성 제품, 초콜릿, 식물성 물질, 생선, 맥아즙, 혈액, 조미료</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>의약품, 신체 부위, 약물 및 식물성 물질을 보관하도록 설계된 소형 선반입니다. 전원이 공급되는 한, 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; \n총 스택 크기: 36\n타일당 스택: 18\n\n허용된 아이템: 약품, 식물성 물질, 약물, 뉴트로아민, 신체 부위, 의료 장비\n\n&lt;color=#0094FF&gt;전원이 공급되면 보관된 품목을 냉동할 수 있습니다.&lt;/color&gt;</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대량의 물품과 귀중품을 보관하도록 설계된 나무 상자 모음입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; \n총 스택 크기: 40\n타일당 스택: 10\n\n허용된 아이템: 음식, 시체, 조각을 제외한 모든 것</t>
+  </si>
+  <si>
+    <t>대량의 물품과 귀중품을 보관하도록 설계된 튼튼한 나무 상자입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt; \n총 스택 크기: 8\n타일당 스택: 8\n\n허용된 아이템: 음식, 시체, 조각을 제외한 모든 것</t>
+  </si>
+  <si>
+    <t>건설 및 제작에 사용되는 조각 및 블록을 보관하기 위해 특별히 설계된 작은 더미입니다. 내부에 저장된 아이템은 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 6\n타일당 스택: 6\n\n허용된 아이템: 석재, 조각</t>
+  </si>
+  <si>
+    <t>건설 및 제작에 사용되는 조각 및 블록을 보관하기 위해 특별히 설계된 더 큰 더미입니다. 내부에 저장된 아이템은 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 32\n타일당 스택: 8\n\n허용된 아이템: 석재, 조각</t>
+  </si>
+  <si>
+    <t>돌더미</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>대형 돌더미</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>건설, 제작 및 연료용으로 사용되는 통나무를 보관하기 위해 특별히 설계된 작은 더미입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 6\n타일당 스택: 6\n\n허용된 아이템: 나무</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>건설, 제작 및 연료용으로 사용되는 통나무를 보관하기 위해 특별히 설계된 더 큰 더미입니다. 내부에 저장된 아이템은 시간이 지나도 손상되지 않으며 주변의 미관에 영향을 미치지 않습니다.\n\n&lt;color=#E5E54C&gt;저장소 정보:&lt;/color&gt;\n총 스택 크기: 18\n타일당 스택: 6\n\n허용된 아이템: 나무</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1708,17 +1995,12 @@
       <charset val="129"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF87CEEB"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1733,10 +2015,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -2040,10 +2321,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
@@ -2052,8 +2333,8 @@
     <col min="2" max="2" width="19.54296875" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="68.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="72" style="1" customWidth="1"/>
-    <col min="6" max="6" width="41.36328125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="72" style="2" customWidth="1"/>
+    <col min="6" max="6" width="41.36328125" style="2" customWidth="1"/>
     <col min="7" max="7" width="9.1796875" style="1" customWidth="1"/>
     <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
@@ -2071,10 +2352,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -2088,10 +2369,10 @@
       <c r="C2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2105,11 +2386,11 @@
       <c r="C3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
+      <c r="F3" s="2" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.45">
@@ -2122,10 +2403,10 @@
       <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -2139,10 +2420,10 @@
       <c r="C5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2156,10 +2437,10 @@
       <c r="C6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -2173,10 +2454,10 @@
       <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2190,10 +2471,10 @@
       <c r="C8" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -2207,10 +2488,10 @@
       <c r="C9" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2224,10 +2505,10 @@
       <c r="C10" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>358</v>
-      </c>
-      <c r="F10" s="1" t="s">
+      <c r="E10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="2" t="s">
         <v>43</v>
       </c>
     </row>
@@ -2241,11 +2522,11 @@
       <c r="C11" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>47</v>
+      <c r="F11" s="2" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.45">
@@ -2258,10 +2539,10 @@
       <c r="C12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="F12" s="1" t="s">
+      <c r="E12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>51</v>
       </c>
     </row>
@@ -2275,11 +2556,11 @@
       <c r="C13" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>55</v>
+      <c r="F13" s="2" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.45">
@@ -2292,11 +2573,11 @@
       <c r="C14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>59</v>
+      <c r="E14" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>529</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.45">
@@ -2309,11 +2590,11 @@
       <c r="C15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="F15" s="1" t="s">
-        <v>63</v>
+      <c r="F15" s="2" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.45">
@@ -2326,10 +2607,10 @@
       <c r="C16" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="F16" s="1" t="s">
+      <c r="E16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2343,11 +2624,11 @@
       <c r="C17" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>71</v>
+      <c r="F17" s="2" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.45">
@@ -2360,10 +2641,10 @@
       <c r="C18" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="E18" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>75</v>
       </c>
     </row>
@@ -2377,11 +2658,11 @@
       <c r="C19" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F19" s="1" t="s">
-        <v>79</v>
+      <c r="F19" s="2" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.45">
@@ -2394,10 +2675,10 @@
       <c r="C20" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="F20" s="1" t="s">
+      <c r="E20" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>83</v>
       </c>
     </row>
@@ -2411,11 +2692,11 @@
       <c r="C21" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>87</v>
+      <c r="F21" s="2" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.45">
@@ -2428,11 +2709,11 @@
       <c r="C22" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>91</v>
+      <c r="E22" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.45">
@@ -2445,11 +2726,11 @@
       <c r="C23" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="E23" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>95</v>
+      <c r="F23" s="2" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.45">
@@ -2462,10 +2743,10 @@
       <c r="C24" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F24" s="1" t="s">
+      <c r="E24" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2479,11 +2760,11 @@
       <c r="C25" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E25" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F25" s="1" t="s">
-        <v>103</v>
+      <c r="F25" s="2" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.45">
@@ -2496,10 +2777,10 @@
       <c r="C26" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F26" s="1" t="s">
+      <c r="E26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F26" s="2" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2513,11 +2794,11 @@
       <c r="C27" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="E27" s="3" t="s">
+      <c r="E27" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="F27" s="1" t="s">
-        <v>375</v>
+      <c r="F27" s="2" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -2530,10 +2811,10 @@
       <c r="C28" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F28" s="1" t="s">
+      <c r="E28" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="2" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2547,11 +2828,11 @@
       <c r="C29" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>118</v>
+      <c r="E29" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.45">
@@ -2564,11 +2845,11 @@
       <c r="C30" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>122</v>
+      <c r="E30" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>530</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.45">
@@ -2581,11 +2862,11 @@
       <c r="C31" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="E31" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="F31" s="1" t="s">
-        <v>126</v>
+      <c r="F31" s="2" t="s">
+        <v>528</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.45">
@@ -2598,11 +2879,11 @@
       <c r="C32" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>130</v>
+      <c r="E32" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.45">
@@ -2615,11 +2896,11 @@
       <c r="C33" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F33" s="1" t="s">
-        <v>134</v>
+      <c r="F33" s="2" t="s">
+        <v>532</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.45">
@@ -2632,10 +2913,10 @@
       <c r="C34" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F34" s="1" t="s">
+      <c r="E34" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>138</v>
       </c>
     </row>
@@ -2649,11 +2930,11 @@
       <c r="C35" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>142</v>
+      <c r="F35" s="2" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.45">
@@ -2666,10 +2947,10 @@
       <c r="C36" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="F36" s="1" t="s">
+      <c r="E36" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>146</v>
       </c>
     </row>
@@ -2683,11 +2964,11 @@
       <c r="C37" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="E37" s="3" t="s">
+      <c r="E37" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>150</v>
+      <c r="F37" s="2" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.45">
@@ -2700,10 +2981,10 @@
       <c r="C38" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="F38" s="1" t="s">
+      <c r="E38" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="F38" s="2" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2717,11 +2998,11 @@
       <c r="C39" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="F39" s="1" t="s">
-        <v>158</v>
+      <c r="F39" s="2" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.45">
@@ -2734,16 +3015,16 @@
       <c r="C40" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="F40" s="1" t="s">
-        <v>163</v>
+      <c r="E40" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>40</v>
@@ -2751,11 +3032,11 @@
       <c r="C41" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="E41" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="F41" s="1" t="s">
-        <v>166</v>
+      <c r="F41" s="2" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.45">
@@ -2768,10 +3049,10 @@
       <c r="C42" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="F42" s="1" t="s">
+      <c r="E42" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="F42" s="2" t="s">
         <v>170</v>
       </c>
     </row>
@@ -2785,11 +3066,11 @@
       <c r="C43" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>174</v>
+      <c r="E43" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.45">
@@ -2802,10 +3083,10 @@
       <c r="C44" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="F44" s="1" t="s">
+      <c r="E44" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="F44" s="2" t="s">
         <v>178</v>
       </c>
     </row>
@@ -2819,11 +3100,11 @@
       <c r="C45" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F45" s="1" t="s">
-        <v>182</v>
+      <c r="F45" s="2" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.45">
@@ -2836,10 +3117,10 @@
       <c r="C46" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>177</v>
-      </c>
-      <c r="F46" s="1" t="s">
+      <c r="E46" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="F46" s="2" t="s">
         <v>186</v>
       </c>
     </row>
@@ -2853,11 +3134,11 @@
       <c r="C47" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="E47" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>190</v>
+      <c r="F47" s="2" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.45">
@@ -2870,11 +3151,11 @@
       <c r="C48" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>185</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>194</v>
+      <c r="E48" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.45">
@@ -2887,11 +3168,11 @@
       <c r="C49" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>197</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>198</v>
+      <c r="E49" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.45">
@@ -2904,10 +3185,10 @@
       <c r="C50" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="F50" s="1" t="s">
+      <c r="E50" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F50" s="2" t="s">
         <v>202</v>
       </c>
     </row>
@@ -2921,11 +3202,11 @@
       <c r="C51" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E51" s="3" t="s">
+      <c r="E51" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="F51" s="1" t="s">
-        <v>206</v>
+      <c r="F51" s="2" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.45">
@@ -2938,11 +3219,11 @@
       <c r="C52" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E52" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>210</v>
+      <c r="E52" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.45">
@@ -2955,11 +3236,11 @@
       <c r="C53" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="F53" s="1" t="s">
-        <v>214</v>
+      <c r="F53" s="2" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.45">
@@ -2972,10 +3253,10 @@
       <c r="C54" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="F54" s="1" t="s">
+      <c r="E54" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="F54" s="2" t="s">
         <v>218</v>
       </c>
     </row>
@@ -2989,11 +3270,11 @@
       <c r="C55" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="E55" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="F55" s="1" t="s">
-        <v>222</v>
+      <c r="F55" s="2" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.45">
@@ -3006,10 +3287,10 @@
       <c r="C56" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="E56" s="3" t="s">
-        <v>217</v>
-      </c>
-      <c r="F56" s="1" t="s">
+      <c r="E56" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="F56" s="2" t="s">
         <v>226</v>
       </c>
     </row>
@@ -3023,11 +3304,11 @@
       <c r="C57" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>225</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>392</v>
+      <c r="E57" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
@@ -3040,10 +3321,10 @@
       <c r="C58" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="F58" s="1" t="s">
+      <c r="E58" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="F58" s="2" t="s">
         <v>233</v>
       </c>
     </row>
@@ -3057,11 +3338,11 @@
       <c r="C59" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="E59" s="3" t="s">
+      <c r="E59" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="F59" s="1" t="s">
-        <v>237</v>
+      <c r="F59" s="2" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.45">
@@ -3074,10 +3355,10 @@
       <c r="C60" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E60" s="3" t="s">
-        <v>232</v>
-      </c>
-      <c r="F60" s="1" t="s">
+      <c r="E60" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="F60" s="2" t="s">
         <v>241</v>
       </c>
     </row>
@@ -3091,11 +3372,11 @@
       <c r="C61" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="E61" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="F61" s="1" t="s">
-        <v>245</v>
+      <c r="F61" s="2" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.45">
@@ -3108,10 +3389,10 @@
       <c r="C62" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E62" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="F62" s="1" t="s">
+      <c r="E62" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="F62" s="2" t="s">
         <v>249</v>
       </c>
     </row>
@@ -3125,11 +3406,11 @@
       <c r="C63" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="E63" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="F63" s="1" t="s">
-        <v>253</v>
+      <c r="F63" s="2" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.45">
@@ -3142,10 +3423,10 @@
       <c r="C64" s="1" t="s">
         <v>255</v>
       </c>
-      <c r="E64" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="F64" s="1" t="s">
+      <c r="E64" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="F64" s="2" t="s">
         <v>257</v>
       </c>
     </row>
@@ -3159,11 +3440,11 @@
       <c r="C65" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="E65" s="3" t="s">
+      <c r="E65" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="F65" s="1" t="s">
-        <v>365</v>
+      <c r="F65" s="2" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
@@ -3176,10 +3457,10 @@
       <c r="C66" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="E66" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="F66" s="1" t="s">
+      <c r="E66" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="F66" s="2" t="s">
         <v>264</v>
       </c>
     </row>
@@ -3193,11 +3474,11 @@
       <c r="C67" s="1" t="s">
         <v>266</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="E67" s="2" t="s">
         <v>267</v>
       </c>
-      <c r="F67" s="1" t="s">
-        <v>393</v>
+      <c r="F67" s="2" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
@@ -3208,590 +3489,616 @@
         <v>269</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>397</v>
+        <v>271</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>395</v>
-      </c>
-      <c r="E69" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>396</v>
+        <v>274</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F69" s="2" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>273</v>
+        <v>292</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>274</v>
+        <v>294</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E70" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>364</v>
+        <v>295</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>296</v>
+      </c>
+      <c r="F70" s="2" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>277</v>
+        <v>297</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>278</v>
+        <v>299</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>389</v>
+        <v>295</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>280</v>
+        <v>301</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>281</v>
+        <v>302</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E72" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>366</v>
+        <v>295</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>285</v>
+        <v>306</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>367</v>
+        <v>295</v>
+      </c>
+      <c r="E73" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="F73" s="2" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>287</v>
+        <v>308</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>288</v>
+        <v>309</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>368</v>
+        <v>295</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="F74" s="2" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
-        <v>291</v>
+        <v>311</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>292</v>
+        <v>313</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>369</v>
+        <v>295</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="F75" s="2" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
-        <v>294</v>
+        <v>373</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>295</v>
+        <v>375</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>370</v>
+        <v>376</v>
+      </c>
+      <c r="E76" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="F76" s="2" t="s">
+        <v>378</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
-        <v>297</v>
+        <v>379</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>298</v>
+        <v>380</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>371</v>
+        <v>376</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>381</v>
+      </c>
+      <c r="F77" s="2" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
-        <v>300</v>
+        <v>382</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>301</v>
+        <v>383</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>372</v>
+        <v>384</v>
+      </c>
+      <c r="E78" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
-        <v>303</v>
+        <v>387</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>304</v>
+        <v>388</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>289</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>373</v>
+        <v>384</v>
+      </c>
+      <c r="E79" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="F79" s="2" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
-        <v>306</v>
+        <v>390</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>307</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E80" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>374</v>
+        <v>351</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F80" s="2" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
-        <v>310</v>
+        <v>348</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="D81" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E81" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>376</v>
+        <v>343</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="F81" s="2" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
-        <v>313</v>
+        <v>335</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>314</v>
-      </c>
-      <c r="D82" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E82" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>377</v>
+        <v>331</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>317</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E83" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>381</v>
+        <v>324</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
-        <v>319</v>
+        <v>293</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>320</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E84" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>378</v>
+        <v>289</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
-        <v>322</v>
+        <v>279</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>323</v>
-      </c>
-      <c r="D85" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E85" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>398</v>
+        <v>427</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>428</v>
+      </c>
+      <c r="F85" s="2" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
-        <v>325</v>
+        <v>429</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>379</v>
+        <v>430</v>
+      </c>
+      <c r="E86" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
-        <v>328</v>
+        <v>431</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>329</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>399</v>
+        <v>432</v>
+      </c>
+      <c r="E87" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="F87" s="2" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
-        <v>331</v>
+        <v>434</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>332</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>380</v>
+        <v>435</v>
+      </c>
+      <c r="E88" s="2" t="s">
+        <v>436</v>
+      </c>
+      <c r="F88" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
-        <v>334</v>
+        <v>437</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>308</v>
-      </c>
-      <c r="E89" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>400</v>
+        <v>438</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>525</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
-        <v>337</v>
+        <v>439</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="E90" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>382</v>
+        <v>440</v>
+      </c>
+      <c r="E90" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="F90" s="2" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
-        <v>341</v>
+        <v>442</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>339</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>383</v>
+        <v>443</v>
+      </c>
+      <c r="E91" s="2" t="s">
+        <v>444</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
-        <v>344</v>
+        <v>445</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="E92" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>384</v>
+        <v>446</v>
+      </c>
+      <c r="E92" s="2" t="s">
+        <v>447</v>
+      </c>
+      <c r="F92" s="2" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
-        <v>348</v>
+        <v>448</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="D93" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="E93" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>385</v>
+        <v>449</v>
+      </c>
+      <c r="E93" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
-        <v>351</v>
+        <v>451</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="E94" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>386</v>
+        <v>452</v>
+      </c>
+      <c r="E94" s="2" t="s">
+        <v>453</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
-        <v>355</v>
+        <v>454</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>269</v>
+        <v>40</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="D95" s="1" t="s">
-        <v>353</v>
-      </c>
-      <c r="E95" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>387</v>
+        <v>455</v>
+      </c>
+      <c r="E95" s="2" t="s">
+        <v>450</v>
+      </c>
+      <c r="F95" s="2" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A96" s="1" t="s">
-        <v>263</v>
+        <v>456</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="D96" s="1" t="s">
-        <v>360</v>
+        <v>457</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>361</v>
+        <v>129</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>388</v>
+        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A97" s="1" t="s">
-        <v>362</v>
+        <v>458</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="D97" s="1" t="s">
-        <v>360</v>
-      </c>
-      <c r="E97" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="F97" s="1" t="s">
-        <v>390</v>
+        <v>459</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A98" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="B98" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A99" s="1" t="s">
+        <v>464</v>
+      </c>
+      <c r="B99" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="E99" s="2" t="s">
+        <v>466</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A100" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="B100" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A101" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="B101" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>295</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>472</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>513</v>
       </c>
     </row>
   </sheetData>
@@ -3816,7 +4123,8 @@
     <col min="4" max="4" width="68.90625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53.08984375" style="1" customWidth="1"/>
     <col min="6" max="6" width="41.36328125" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.1796875" style="1"/>
+    <col min="7" max="7" width="9.1796875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
@@ -3986,7 +4294,7 @@
         <v>41</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>439</v>
+        <v>389</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>43</v>
@@ -4020,7 +4328,7 @@
         <v>49</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>438</v>
+        <v>391</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>51</v>
@@ -4054,7 +4362,7 @@
         <v>57</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>437</v>
+        <v>392</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>59</v>
@@ -4088,7 +4396,7 @@
         <v>65</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>436</v>
+        <v>393</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>67</v>
@@ -4122,7 +4430,7 @@
         <v>73</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>435</v>
+        <v>394</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>75</v>
@@ -4156,7 +4464,7 @@
         <v>81</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>434</v>
+        <v>395</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>83</v>
@@ -4190,7 +4498,7 @@
         <v>89</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>433</v>
+        <v>396</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>91</v>
@@ -4224,7 +4532,7 @@
         <v>97</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>432</v>
+        <v>397</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>99</v>
@@ -4278,7 +4586,7 @@
         <v>110</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>431</v>
+        <v>398</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.45">
@@ -4292,7 +4600,7 @@
         <v>112</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>430</v>
+        <v>399</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>114</v>
@@ -4309,7 +4617,7 @@
         <v>116</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>429</v>
+        <v>400</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>118</v>
@@ -4326,7 +4634,7 @@
         <v>120</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>428</v>
+        <v>401</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>122</v>
@@ -4360,7 +4668,7 @@
         <v>128</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>427</v>
+        <v>402</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>130</v>
@@ -4394,7 +4702,7 @@
         <v>136</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>426</v>
+        <v>403</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>138</v>
@@ -4428,7 +4736,7 @@
         <v>144</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>425</v>
+        <v>404</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>146</v>
@@ -4462,7 +4770,7 @@
         <v>152</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>424</v>
+        <v>405</v>
       </c>
       <c r="F38" s="1" t="s">
         <v>154</v>
@@ -4496,15 +4804,15 @@
         <v>160</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>423</v>
+        <v>406</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>422</v>
+        <v>162</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A41" s="1" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>40</v>
@@ -4530,7 +4838,7 @@
         <v>168</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>421</v>
+        <v>408</v>
       </c>
       <c r="F42" s="1" t="s">
         <v>170</v>
@@ -4547,7 +4855,7 @@
         <v>172</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="F43" s="1" t="s">
         <v>174</v>
@@ -4564,7 +4872,7 @@
         <v>176</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>419</v>
+        <v>409</v>
       </c>
       <c r="F44" s="1" t="s">
         <v>178</v>
@@ -4598,7 +4906,7 @@
         <v>184</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>418</v>
+        <v>410</v>
       </c>
       <c r="F46" s="1" t="s">
         <v>186</v>
@@ -4632,7 +4940,7 @@
         <v>192</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>417</v>
+        <v>411</v>
       </c>
       <c r="F48" s="1" t="s">
         <v>194</v>
@@ -4666,7 +4974,7 @@
         <v>200</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="F50" s="1" t="s">
         <v>202</v>
@@ -4700,7 +5008,7 @@
         <v>208</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="F52" s="1" t="s">
         <v>210</v>
@@ -4768,7 +5076,7 @@
         <v>224</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="F56" s="1" t="s">
         <v>226</v>
@@ -4785,10 +5093,10 @@
         <v>228</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>411</v>
+        <v>417</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.45">
@@ -4802,7 +5110,7 @@
         <v>231</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>410</v>
+        <v>418</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>233</v>
@@ -4836,7 +5144,7 @@
         <v>239</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>409</v>
+        <v>419</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>241</v>
@@ -4870,7 +5178,7 @@
         <v>247</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>408</v>
+        <v>420</v>
       </c>
       <c r="F62" s="1" t="s">
         <v>249</v>
@@ -4904,7 +5212,7 @@
         <v>255</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>407</v>
+        <v>421</v>
       </c>
       <c r="F64" s="1" t="s">
         <v>257</v>
@@ -4924,7 +5232,7 @@
         <v>260</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>406</v>
+        <v>422</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.45">
@@ -4938,7 +5246,7 @@
         <v>262</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>405</v>
+        <v>423</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>264</v>
@@ -4958,7 +5266,7 @@
         <v>267</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>404</v>
+        <v>424</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.45">
@@ -4969,550 +5277,466 @@
         <v>269</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>403</v>
+        <v>425</v>
       </c>
       <c r="E68" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="F68" s="1" t="s">
-        <v>401</v>
-      </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A69" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>402</v>
+        <v>426</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>272</v>
-      </c>
-      <c r="F69" s="1" t="s">
-        <v>401</v>
+        <v>273</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A70" s="1" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>401</v>
+        <v>278</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A71" s="1" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>279</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>401</v>
+        <v>282</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A72" s="1" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="F72" s="1" t="s">
-        <v>401</v>
+        <v>287</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A73" s="1" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>282</v>
+        <v>286</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>286</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>401</v>
+        <v>291</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A74" s="1" t="s">
-        <v>287</v>
+        <v>292</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>290</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>401</v>
+        <v>296</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A75" s="1" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>293</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>401</v>
+        <v>300</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>302</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="D76" s="1" t="s">
-        <v>289</v>
-      </c>
       <c r="E76" s="1" t="s">
-        <v>296</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>401</v>
+        <v>303</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A77" s="1" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>401</v>
+        <v>307</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
-        <v>300</v>
+        <v>308</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>301</v>
+        <v>309</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>302</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>401</v>
+        <v>310</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A79" s="1" t="s">
-        <v>303</v>
+        <v>311</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>401</v>
+        <v>314</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A80" s="1" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>309</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A81" s="1" t="s">
-        <v>310</v>
+        <v>320</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>311</v>
+        <v>321</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>312</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A82" s="1" t="s">
-        <v>313</v>
+        <v>323</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>314</v>
+        <v>325</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A83" s="1" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C83" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>317</v>
       </c>
-      <c r="D83" s="1" t="s">
-        <v>308</v>
-      </c>
       <c r="E83" s="1" t="s">
-        <v>318</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A84" s="1" t="s">
-        <v>319</v>
+        <v>332</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>320</v>
+        <v>333</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>321</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A85" s="1" t="s">
-        <v>322</v>
+        <v>336</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>323</v>
+        <v>337</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>324</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A86" s="1" t="s">
-        <v>325</v>
+        <v>339</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>326</v>
+        <v>341</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>327</v>
-      </c>
-      <c r="F86" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A87" s="1" t="s">
-        <v>328</v>
+        <v>344</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>329</v>
+        <v>345</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>330</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A88" s="1" t="s">
-        <v>331</v>
+        <v>347</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>332</v>
+        <v>349</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>333</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A89" s="1" t="s">
-        <v>334</v>
+        <v>352</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>335</v>
+        <v>353</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>336</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A90" s="1" t="s">
-        <v>337</v>
+        <v>355</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>338</v>
+        <v>357</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>339</v>
+        <v>358</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A91" s="1" t="s">
-        <v>341</v>
+        <v>360</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>342</v>
+        <v>362</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>339</v>
+        <v>358</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A92" s="1" t="s">
-        <v>344</v>
+        <v>364</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>345</v>
+        <v>366</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>346</v>
+        <v>367</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="F92" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A93" s="1" t="s">
-        <v>348</v>
+        <v>370</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>349</v>
+        <v>371</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>346</v>
+        <v>367</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>350</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A94" s="1" t="s">
-        <v>351</v>
+        <v>373</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>352</v>
+        <v>375</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>353</v>
+        <v>376</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="F94" s="1" t="s">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A95" s="1" t="s">
-        <v>355</v>
+        <v>379</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>269</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>356</v>
+        <v>380</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>353</v>
+        <v>376</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>357</v>
-      </c>
-      <c r="F95" s="1" t="s">
-        <v>401</v>
+        <v>381</v>
       </c>
     </row>
   </sheetData>

</xml_diff>